<commit_message>
Accounts functionality and more
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/data.xlsx
+++ b/src/test/resources/TestData/data.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538DAFB2-71DB-49BC-9706-3928E6427BE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>TCName</t>
   </si>
@@ -52,13 +53,46 @@
   </si>
   <si>
     <t>USA</t>
+  </si>
+  <si>
+    <t>Create Account with mandatory_fields_TC04</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Bank of India</t>
+  </si>
+  <si>
+    <t>Login With Theam_TC05</t>
+  </si>
+  <si>
+    <t>Theme</t>
+  </si>
+  <si>
+    <t>nature</t>
+  </si>
+  <si>
+    <t>Potential_Name</t>
+  </si>
+  <si>
+    <t>Sales_Stave</t>
+  </si>
+  <si>
+    <t>Needs Analysis</t>
+  </si>
+  <si>
+    <t>Create potential with mandatory fields_TC06</t>
+  </si>
+  <si>
+    <t>CRM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,6 +103,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -116,10 +157,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -129,6 +172,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -177,7 +223,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -210,9 +256,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -245,6 +308,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -420,19 +500,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.54296875" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,48 +529,103 @@
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <v>12345</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="H7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -499,24 +635,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>